<commit_message>
target radius = 12
</commit_message>
<xml_diff>
--- a/conditions_aftereffect.xlsx
+++ b/conditions_aftereffect.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PSYCHOPY\eyehand_baseline\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B09296D7-B7B3-415C-91D8-F5BB42863B32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E937B920-06C0-46CB-A43A-F921A9B08233}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="1815" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38295" yWindow="1935" windowWidth="14610" windowHeight="15585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -403,7 +403,7 @@
   <dimension ref="A1:C31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.25"/>
@@ -421,7 +421,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B2">
         <v>0</v>
@@ -435,7 +435,7 @@
         <v>0</v>
       </c>
       <c r="B3">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="C3">
         <v>1</v>
@@ -443,10 +443,10 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>11.314</v>
+        <v>8.4849999999999994</v>
       </c>
       <c r="B4">
-        <v>11.314</v>
+        <v>8.4849999999999994</v>
       </c>
       <c r="C4">
         <v>1</v>
@@ -454,10 +454,10 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>-11.314</v>
+        <v>-8.4849999999999994</v>
       </c>
       <c r="B5">
-        <v>11.314</v>
+        <v>8.4849999999999994</v>
       </c>
       <c r="C5">
         <v>1</v>
@@ -465,7 +465,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>-16</v>
+        <v>-12</v>
       </c>
       <c r="B6">
         <v>0</v>
@@ -479,7 +479,7 @@
         <v>0</v>
       </c>
       <c r="B7">
-        <v>-16</v>
+        <v>-12</v>
       </c>
       <c r="C7">
         <v>1</v>
@@ -487,10 +487,10 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>-11.314</v>
+        <v>-8.4849999999999994</v>
       </c>
       <c r="B8">
-        <v>-11.314</v>
+        <v>-8.4849999999999994</v>
       </c>
       <c r="C8">
         <v>1</v>
@@ -498,10 +498,10 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>11.314</v>
+        <v>8.4849999999999994</v>
       </c>
       <c r="B9">
-        <v>-11.314</v>
+        <v>-8.4849999999999994</v>
       </c>
       <c r="C9">
         <v>1</v>
@@ -509,10 +509,10 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>11.314</v>
+        <v>8.4849999999999994</v>
       </c>
       <c r="B10">
-        <v>11.314</v>
+        <v>8.4849999999999994</v>
       </c>
       <c r="C10">
         <v>1</v>
@@ -520,7 +520,7 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B11">
         <v>0</v>
@@ -534,7 +534,7 @@
         <v>0</v>
       </c>
       <c r="B12">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="C12">
         <v>1</v>
@@ -542,7 +542,7 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>-16</v>
+        <v>-12</v>
       </c>
       <c r="B13">
         <v>0</v>
@@ -553,10 +553,10 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>-11.314</v>
+        <v>-8.4849999999999994</v>
       </c>
       <c r="B14">
-        <v>11.314</v>
+        <v>8.4849999999999994</v>
       </c>
       <c r="C14">
         <v>1</v>
@@ -564,10 +564,10 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>-11.314</v>
+        <v>-8.4849999999999994</v>
       </c>
       <c r="B15">
-        <v>-11.314</v>
+        <v>-8.4849999999999994</v>
       </c>
       <c r="C15">
         <v>1</v>
@@ -578,7 +578,7 @@
         <v>0</v>
       </c>
       <c r="B16">
-        <v>-16</v>
+        <v>-12</v>
       </c>
       <c r="C16">
         <v>1</v>
@@ -586,10 +586,10 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17">
-        <v>11.314</v>
+        <v>8.4849999999999994</v>
       </c>
       <c r="B17">
-        <v>-11.314</v>
+        <v>8.4849999999999994</v>
       </c>
       <c r="C17">
         <v>1</v>
@@ -600,7 +600,7 @@
         <v>0</v>
       </c>
       <c r="B18">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="C18">
         <v>1</v>
@@ -608,10 +608,10 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19">
-        <v>11.314</v>
+        <v>8.4849999999999994</v>
       </c>
       <c r="B19">
-        <v>11.314</v>
+        <v>8.4849999999999994</v>
       </c>
       <c r="C19">
         <v>1</v>
@@ -619,7 +619,7 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B20">
         <v>0</v>
@@ -630,10 +630,10 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21">
-        <v>-11.314</v>
+        <v>-8.4849999999999994</v>
       </c>
       <c r="B21">
-        <v>11.314</v>
+        <v>8.4849999999999994</v>
       </c>
       <c r="C21">
         <v>1</v>
@@ -641,7 +641,7 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22">
-        <v>-16</v>
+        <v>-12</v>
       </c>
       <c r="B22">
         <v>0</v>
@@ -652,10 +652,10 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23">
-        <v>-11.314</v>
+        <v>-8.4849999999999994</v>
       </c>
       <c r="B23">
-        <v>-11.314</v>
+        <v>-8.4849999999999994</v>
       </c>
       <c r="C23">
         <v>1</v>
@@ -663,10 +663,10 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24">
-        <v>11.314</v>
+        <v>8.4849999999999994</v>
       </c>
       <c r="B24">
-        <v>-11.314</v>
+        <v>-8.4849999999999994</v>
       </c>
       <c r="C24">
         <v>1</v>
@@ -677,7 +677,7 @@
         <v>0</v>
       </c>
       <c r="B25">
-        <v>-16</v>
+        <v>-12</v>
       </c>
       <c r="C25">
         <v>1</v>
@@ -685,10 +685,10 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26">
-        <v>-11.314</v>
+        <v>-8.4849999999999994</v>
       </c>
       <c r="B26">
-        <v>11.314</v>
+        <v>8.4849999999999994</v>
       </c>
       <c r="C26">
         <v>1</v>
@@ -696,10 +696,10 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27">
-        <v>11.314</v>
+        <v>8.4849999999999994</v>
       </c>
       <c r="B27">
-        <v>11.314</v>
+        <v>8.4849999999999994</v>
       </c>
       <c r="C27">
         <v>1</v>
@@ -710,7 +710,7 @@
         <v>0</v>
       </c>
       <c r="B28">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="C28">
         <v>1</v>
@@ -721,7 +721,7 @@
         <v>0</v>
       </c>
       <c r="B29">
-        <v>-16</v>
+        <v>-12</v>
       </c>
       <c r="C29">
         <v>1</v>
@@ -729,7 +729,7 @@
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30">
-        <v>-16</v>
+        <v>-12</v>
       </c>
       <c r="B30">
         <v>0</v>
@@ -740,10 +740,10 @@
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31">
-        <v>-11.314</v>
+        <v>-8.4849999999999994</v>
       </c>
       <c r="B31">
-        <v>-11.314</v>
+        <v>-8.4849999999999994</v>
       </c>
       <c r="C31">
         <v>1</v>

</xml_diff>